<commit_message>
first outline of exercises
</commit_message>
<xml_diff>
--- a/Annual2017-EU/data/RDFModel.xlsx
+++ b/Annual2017-EU/data/RDFModel.xlsx
@@ -5,18 +5,17 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_sandbox\PhUSE\Annual\2017\workshop\Exercises\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_gitHub\LinkedDataWorkshop\Annual2017-EU\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6950"/>
   </bookViews>
   <sheets>
-    <sheet name="RDFModel" sheetId="1" r:id="rId1"/>
-    <sheet name="Lists" sheetId="2" r:id="rId2"/>
+    <sheet name="Neo4jModel" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="DataTypes">Lists!$A$2:$A$5</definedName>
+    <definedName name="DataTypes">#REF!</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
@@ -28,50 +27,20 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="17">
-  <si>
-    <t>Subject</t>
-  </si>
-  <si>
-    <t>Predicate</t>
-  </si>
-  <si>
-    <t>Object</t>
-  </si>
-  <si>
-    <t>ObjectType</t>
-  </si>
-  <si>
-    <t>hasAge</t>
-  </si>
-  <si>
-    <t>int</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="23">
   <si>
     <t>hasTreatment</t>
   </si>
   <si>
-    <t>uri</t>
-  </si>
-  <si>
-    <t>string</t>
-  </si>
-  <si>
     <t>Person1</t>
   </si>
   <si>
-    <t>hasFirstName</t>
-  </si>
-  <si>
     <t>Study1</t>
   </si>
   <si>
     <t>Placebo</t>
   </si>
   <si>
-    <t>Permitted Data Types</t>
-  </si>
-  <si>
     <t>Bob</t>
   </si>
   <si>
@@ -79,13 +48,61 @@
   </si>
   <si>
     <t>participatesIn</t>
+  </si>
+  <si>
+    <t>Node1</t>
+  </si>
+  <si>
+    <t>Relation</t>
+  </si>
+  <si>
+    <t>Node2</t>
+  </si>
+  <si>
+    <t>Treat1</t>
+  </si>
+  <si>
+    <t>Node</t>
+  </si>
+  <si>
+    <t>Parameter</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>firstName</t>
+  </si>
+  <si>
+    <t>age</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>Phase 2 Double-blind study of Serum 114</t>
+  </si>
+  <si>
+    <t>treatment</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>Sugar water</t>
+  </si>
+  <si>
+    <t>Relations</t>
+  </si>
+  <si>
+    <t>Node Parameter:Value Pairs</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -101,8 +118,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -112,12 +144,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -135,12 +161,30 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="-0.249977111117893"/>
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -163,22 +207,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -188,16 +221,24 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -517,232 +558,250 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="16.08984375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.54296875" style="3" customWidth="1"/>
-    <col min="4" max="4" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="36.26953125" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:7" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A1" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="C4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="F4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="5">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="B5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="E6" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="6">
-        <v>32</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E7" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="1"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="2"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="2"/>
-      <c r="D9" s="1"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="2"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="2"/>
-      <c r="D10" s="1"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="2"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="2"/>
-      <c r="D11" s="1"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="1"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="1"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="1"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="1"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="1"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="1"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="1"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="1"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="2"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12" s="13"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="14"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="2"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13" s="13"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="14"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="2"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A14" s="13"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="14"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="2"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A15" s="13"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="14"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="2"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A16" s="13"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="14"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="2"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A17" s="13"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="14"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="2"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A18" s="13"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="14"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="2"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A19" s="13"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="14"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="2"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A20" s="13"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="14"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="14"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A21" s="13"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="14"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="14"/>
     </row>
   </sheetData>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Incorrect Data Type" error="Enter a data type as one of the following:_x000a_int_x000a_string_x000a_uri" sqref="D2">
-      <formula1>DataTypes</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3:D5 D7:D20">
-      <formula1>DataTypes</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
presentation moved to git
</commit_message>
<xml_diff>
--- a/Annual2017-EU/data/RDFModel.xlsx
+++ b/Annual2017-EU/data/RDFModel.xlsx
@@ -229,7 +229,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
@@ -262,6 +262,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyBorder="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -655,7 +658,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -794,69 +799,69 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="4"/>
+      <c r="A10" s="14"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
       <c r="D10" s="2"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="4"/>
+      <c r="A11" s="14"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="14"/>
       <c r="D11" s="2"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="4"/>
+      <c r="A12" s="14"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="14"/>
       <c r="D12" s="2"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="4"/>
+      <c r="A13" s="14"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
       <c r="D13" s="2"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="4"/>
+      <c r="A14" s="14"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
       <c r="D14" s="2"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="4"/>
+      <c r="A15" s="14"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
       <c r="D15" s="2"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="4"/>
+      <c r="A16" s="14"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="14"/>
       <c r="D16" s="2"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="4"/>
+      <c r="A17" s="14"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="14"/>
       <c r="D17" s="2"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="4"/>
+      <c r="A18" s="14"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="14"/>
       <c r="D18" s="2"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="4"/>
+      <c r="A19" s="14"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="14"/>
       <c r="D19" s="2"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="4"/>
+      <c r="A20" s="14"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="14"/>
       <c r="D20" s="2"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
@@ -1040,7 +1045,7 @@
       <c r="D50" s="2"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="7YJtBG3I1WCxwJz8CNhfYmvY60UFtNiiGhU1RnaKGquTuS5kkNTQXw45Q+FsQsRxu9wY6SuthlPp+YaQ0O2phA==" saltValue="kLO+2plwNbNZqZVCQAOxbw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="7Cz37fzzJzDzYlE3GWjuq9CJdYKCfzkesXBU8yx+KPSH8Va4McwTd+hTaRsjS9Z96dVWBaJdgiA5uw8Q2kzPwg==" saltValue="VK56cApzRipTkx9GzM3N+Q==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <conditionalFormatting sqref="D2:D26">
     <cfRule type="cellIs" dxfId="8" priority="7" operator="equal">
       <formula>"uri"</formula>

</xml_diff>